<commit_message>
"Updated Analytics component to fetch data based on selected date, added data fetching and error handling, modified ExportExcel component to handle data and formatting, and updated action to accept date parameter."
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CeyInfo\eliot-rfid-tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CeyInfo\eliot-rfid-tracker\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6080FAA-0846-4124-897E-C25DF91FFF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66172C0E-1036-431C-AF45-770D64412B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{51C2EBEF-390C-451A-9A43-DAB54A3E69F8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Target Vs Achivement</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Apparel Gallery Ltd</t>
+  </si>
+  <si>
+    <t>7 to 8</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -441,65 +444,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -522,12 +483,70 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,7 +800,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>21773</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -839,7 +858,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>10887</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>718457</xdr:rowOff>
@@ -897,7 +916,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
@@ -955,7 +974,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>21772</xdr:rowOff>
@@ -1311,378 +1330,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE41F47-B0BA-4093-BF57-14CD105B14A2}">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="16"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="16"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="32"/>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="32"/>
-      <c r="AD3" s="32"/>
-      <c r="AE3" s="32"/>
-      <c r="AF3" s="32"/>
-      <c r="AG3" s="32"/>
-      <c r="AH3" s="32"/>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
     </row>
-    <row r="4" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:34" ht="21" x14ac:dyDescent="0.5">
-      <c r="A5" s="1" t="s">
+    <row r="4" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:35" ht="21" x14ac:dyDescent="0.5">
+      <c r="A5" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="1" t="s">
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="6"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="30"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10" t="s">
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="N6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="O6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="P6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="Q6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="R6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="S6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="S6" s="14"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="13" t="s">
+      <c r="T6" s="24"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="V6" s="14"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="13" t="s">
+      <c r="W6" s="24"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="13" t="s">
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="13" t="s">
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="7" t="s">
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AE6" s="10" t="s">
+      <c r="AF6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="AF6" s="10" t="s">
+      <c r="AG6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="AG6" s="10" t="s">
+      <c r="AH6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="AH6" s="11" t="s">
+      <c r="AI6" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17" t="s">
+    <row r="7" spans="1:35" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="18"/>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="G7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="H7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="I7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="J7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="K7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="L7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="21" t="s">
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="S7" s="21" t="s">
+      <c r="T7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="T7" s="21" t="s">
+      <c r="U7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="U7" s="21" t="s">
+      <c r="V7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="V7" s="21" t="s">
+      <c r="W7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="W7" s="21" t="s">
+      <c r="X7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="X7" s="21" t="s">
+      <c r="Y7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Y7" s="21" t="s">
+      <c r="Z7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Z7" s="21" t="s">
+      <c r="AA7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AA7" s="21" t="s">
+      <c r="AB7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AB7" s="21" t="s">
+      <c r="AC7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AC7" s="22" t="s">
+      <c r="AD7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AD7" s="16"/>
       <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="18"/>
-      <c r="AH7" s="19"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="22"/>
     </row>
-    <row r="8" spans="1:34" ht="21" x14ac:dyDescent="0.5">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="27"/>
-      <c r="Y8" s="28"/>
-      <c r="Z8" s="27"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="29"/>
-      <c r="AC8" s="30"/>
-      <c r="AD8" s="31"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="24"/>
-      <c r="AG8" s="24"/>
-      <c r="AH8" s="25"/>
+    <row r="8" spans="1:35" ht="21" x14ac:dyDescent="0.5">
+      <c r="A8" s="6"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:AH3"/>
-    <mergeCell ref="AD6:AD7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="A1:AI3"/>
     <mergeCell ref="AE6:AE7"/>
     <mergeCell ref="AF6:AF7"/>
     <mergeCell ref="AG6:AG7"/>
     <mergeCell ref="AH6:AH7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="A5:N5"/>
-    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="AI6:AI7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="A5:O5"/>
+    <mergeCell ref="AE5:AI5"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="C6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>